<commit_message>
parallel process barcode split
</commit_message>
<xml_diff>
--- a/projects/tRNAseq_third-gen/data/AdapterRemoval/merge_stats.xlsx
+++ b/projects/tRNAseq_third-gen/data/AdapterRemoval/merge_stats.xlsx
@@ -16,24 +16,24 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
+    <t>P5_index</t>
+  </si>
+  <si>
+    <t>P7_index</t>
+  </si>
+  <si>
+    <t>P5_index_seq</t>
+  </si>
+  <si>
+    <t>P7_index_seq</t>
+  </si>
+  <si>
     <t>fastq_mate1_filename</t>
   </si>
   <si>
     <t>fastq_mate2_filename</t>
   </si>
   <si>
-    <t>P5_index</t>
-  </si>
-  <si>
-    <t>P7_index</t>
-  </si>
-  <si>
-    <t>P5_index_seq</t>
-  </si>
-  <si>
-    <t>P7_index_seq</t>
-  </si>
-  <si>
     <t>N_pairs</t>
   </si>
   <si>
@@ -43,6 +43,30 @@
     <t>percent_successfully_merged</t>
   </si>
   <si>
+    <t>D501</t>
+  </si>
+  <si>
+    <t>D701</t>
+  </si>
+  <si>
+    <t>D702</t>
+  </si>
+  <si>
+    <t>D703</t>
+  </si>
+  <si>
+    <t>AGGCTATA</t>
+  </si>
+  <si>
+    <t>ATTACTCG</t>
+  </si>
+  <si>
+    <t>TCCGGAGA</t>
+  </si>
+  <si>
+    <t>CGCTCATT</t>
+  </si>
+  <si>
     <t>P1_R1_DSA-10k.fastq.bz2</t>
   </si>
   <si>
@@ -59,30 +83,6 @@
   </si>
   <si>
     <t>P3_R2_DSA-10k.fastq.bz2</t>
-  </si>
-  <si>
-    <t>D501</t>
-  </si>
-  <si>
-    <t>D701</t>
-  </si>
-  <si>
-    <t>D702</t>
-  </si>
-  <si>
-    <t>D703</t>
-  </si>
-  <si>
-    <t>AGGCTATA</t>
-  </si>
-  <si>
-    <t>ATTACTCG</t>
-  </si>
-  <si>
-    <t>TCCGGAGA</t>
-  </si>
-  <si>
-    <t>CGCTCATT</t>
   </si>
 </sst>
 </file>
@@ -483,16 +483,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
@@ -509,22 +509,22 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -541,19 +541,19 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>

</xml_diff>